<commit_message>
Cells with date support through #to_date method
</commit_message>
<xml_diff>
--- a/data/regular_workbook.xlsx
+++ b/data/regular_workbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet number one" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Cell 1 A</t>
   </si>
   <si>
     <t>Cell 2 B</t>
+  </si>
+  <si>
+    <t>Cell 2 C</t>
+  </si>
+  <si>
+    <t>Dato</t>
   </si>
 </sst>
 </file>
@@ -395,25 +401,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
       <c r="B4" s="1">
         <v>41233</v>
       </c>
@@ -432,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>

</xml_diff>

<commit_message>
look up cell values
</commit_message>
<xml_diff>
--- a/data/regular_workbook.xlsx
+++ b/data/regular_workbook.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet number one" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Cell 1 A</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Dato</t>
+  </si>
+  <si>
+    <t>Sheet 2, cell 2 B</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -442,12 +445,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>